<commit_message>
Updated the test procedure to be compliant with Web version
</commit_message>
<xml_diff>
--- a/VeryGoodWeatherApp_TestProcedure.xlsx
+++ b/VeryGoodWeatherApp_TestProcedure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cedric Eicher\Documents\VeryGoodVentures Coding Challenge\VeryGoodWeatherApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF3F523-07D3-4B3E-A8E7-031AEC7B822B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA754F4-4F41-4D74-BC4D-3B705CD2DBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>Expected Result</t>
   </si>
@@ -429,9 +429,6 @@
   </si>
   <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>1. The app is opened in the emulator or on a physical device</t>
   </si>
   <si>
     <t>2. The user has not interacted with the app yet</t>
@@ -1493,6 +1490,15 @@
       </rPr>
       <t>(see below).</t>
     </r>
+  </si>
+  <si>
+    <t>1. The app is opened either in the Android emulator, the web, or a physical device</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>1. If on Web, ignore all results related to the keyboard.</t>
   </si>
 </sst>
 </file>
@@ -1740,7 +1746,7 @@
       </gradientFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1772,15 +1778,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1798,51 +1827,102 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2132,520 +2212,637 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="56.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="83.42578125" customWidth="1"/>
     <col min="4" max="4" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="7"/>
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="25" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>11</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>14</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>17</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>18</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>20</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>21</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>24</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>25</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>4</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="195" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>5</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>8</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <v>9</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>10</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>11</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="195" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
-        <v>12</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
-        <v>13</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
-        <v>14</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>15</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
-        <v>16</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="210" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
-        <v>17</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
-        <v>18</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
-        <v>19</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
-        <v>20</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
-        <v>21</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
-        <v>22</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
-        <v>23</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="39"/>
+      <c r="E40" s="7"/>
+    </row>
+    <row r="41" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
-        <v>24</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
-        <v>25</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="24"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="12" t="s">
+      <c r="D41" s="19"/>
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C42" s="36" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="12" t="s">
+      <c r="D42" s="37"/>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C43" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="35"/>
+      <c r="E43" s="7"/>
+    </row>
+    <row r="44" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="33"/>
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" s="31"/>
+      <c r="E45" s="7"/>
+    </row>
+    <row r="46" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="29"/>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="27"/>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="25"/>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-      <c r="B46" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="20" t="s">
+      <c r="D49" s="23"/>
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>55</v>
-      </c>
+      <c r="D50" s="21"/>
+      <c r="E50" s="7"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B37:C37"/>
+  <mergeCells count="20">
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B39:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>